<commit_message>
Added files for efast_tightened (original formulation).
</commit_message>
<xml_diff>
--- a/dithionite_sensitivity/parameters.xlsx
+++ b/dithionite_sensitivity/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="883" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="883" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -169,7 +169,7 @@
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -229,6 +229,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF420E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -278,7 +286,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,7 +327,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -788,7 +800,7 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -1027,8 +1039,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1116,17 +1128,17 @@
         <f aca="false">mads!A5</f>
         <v>fraction</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <f aca="false">LOG10(summary!B5)</f>
-        <v>-0.301029995663981</v>
+      <c r="B5" s="10" t="n">
+        <f aca="false">LOG10(0.6)</f>
+        <v>-0.221848749616356</v>
       </c>
       <c r="C5" s="9" t="n">
         <f aca="false">B5-F2</f>
-        <v>-0.401029995663981</v>
-      </c>
-      <c r="D5" s="10" t="n">
+        <v>-0.321848749616356</v>
+      </c>
+      <c r="D5" s="11" t="n">
         <f aca="false">B5+F2</f>
-        <v>-0.201029995663981</v>
+        <v>-0.121848749616356</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed itol and fraction.
</commit_message>
<xml_diff>
--- a/dithionite_sensitivity/parameters.xlsx
+++ b/dithionite_sensitivity/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="883" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,151 +13,156 @@
     <sheet name="mads_tightened" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
-    <t>base</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>k_s2o4_disp</t>
-  </si>
-  <si>
-    <t>/s</t>
-  </si>
-  <si>
-    <t>k_s2o4_o2</t>
-  </si>
-  <si>
-    <t>L^1.5 mol^-1.5 s^-</t>
-  </si>
-  <si>
-    <t>k_s2o4_fe3 x SSA</t>
-  </si>
-  <si>
-    <t>g_sed g_fe(oh)3^- s^-</t>
-  </si>
-  <si>
-    <t>these are kept separate in the code, min and max should be multiplied by 175 for the paper</t>
-  </si>
-  <si>
-    <t>fraction</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>k_fe2_o2_fast</t>
-  </si>
-  <si>
-    <t>g mol^-1 s^-1</t>
-  </si>
-  <si>
-    <t>factor_k_fe2_o2_slow</t>
-  </si>
-  <si>
-    <t>k_fe2_o2_slow</t>
-  </si>
-  <si>
-    <t>k_fe2_cr6_fast</t>
-  </si>
-  <si>
-    <t>factor_k_fe2_cr6_slow</t>
-  </si>
-  <si>
-    <t>k_fe2_cr6_slow</t>
-  </si>
-  <si>
-    <t>is2o4</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>ifeoh3_wt%</t>
-  </si>
-  <si>
-    <t>Wt %</t>
-  </si>
-  <si>
-    <t>must convert to volume fraction</t>
-  </si>
-  <si>
-    <t>ifeoh3_vf</t>
-  </si>
-  <si>
-    <t>M^3/m^3_bulk</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>m/d</t>
-  </si>
-  <si>
-    <t>must convert to darcy velocity</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>Constants for VF calculation</t>
-  </si>
-  <si>
-    <t>rho_bulk</t>
-  </si>
-  <si>
-    <t>kg/m^3</t>
-  </si>
-  <si>
-    <t>mv_feoh3</t>
-  </si>
-  <si>
-    <t>cm^3/mole</t>
-  </si>
-  <si>
-    <t>mw_feoh3</t>
-  </si>
-  <si>
-    <t>g/mole</t>
-  </si>
-  <si>
-    <t>Constants for flow rate</t>
-  </si>
-  <si>
-    <t>phi</t>
-  </si>
-  <si>
-    <t>parameter</t>
-  </si>
-  <si>
-    <t>init</t>
-  </si>
-  <si>
-    <t>k_s2o4_fe3</t>
-  </si>
-  <si>
-    <t>**cannot have fraction &gt; 1</t>
-  </si>
-  <si>
-    <t>ifeoh3</t>
-  </si>
-  <si>
-    <t>Factor</t>
+    <t xml:space="preserve">base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_s2o4_disp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_s2o4_o2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L^1.5 mol^-1.5 s^-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_s2o4_fe3 x SSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g_sed g_fe(oh)3^- s^-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">these are kept separate in the code, min and max should be multiplied by 175 for the paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_fe2_o2_fast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g mol^-1 s^-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor_k_fe2_o2_slow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_fe2_o2_slow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_fe2_cr6_fast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor_k_fe2_cr6_slow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_fe2_cr6_slow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is2o4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifeoh3_wt%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wt %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">must convert to volume fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifeoh3_vf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M^3/m^3_bulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m/d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">must convert to darcy velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constants for VF calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho_bulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg/m^3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mv_feoh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cm^3/mole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mw_feoh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g/mole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constants for flow rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">init</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_s2o4_fe3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**cannot have fraction &gt; 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifeoh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factor</t>
   </si>
 </sst>
 </file>
@@ -165,11 +170,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -222,14 +227,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF420E"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFF420E"/>
       <name val="Arial"/>
@@ -331,7 +328,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -415,15 +412,15 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,13 +798,13 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,13 +1037,13 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,16 +1126,16 @@
         <v>fraction</v>
       </c>
       <c r="B5" s="10" t="n">
-        <f aca="false">LOG10(0.6)</f>
-        <v>-0.221848749616356</v>
+        <f aca="false">LOG10(summary!B5)</f>
+        <v>-0.301029995663981</v>
       </c>
       <c r="C5" s="9" t="n">
         <f aca="false">B5-F2</f>
-        <v>-0.321848749616356</v>
+        <v>-0.401029995663981</v>
       </c>
       <c r="D5" s="11" t="n">
         <f aca="false">B5+F2</f>
-        <v>-0.121848749616356</v>
+        <v>-0.201029995663981</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updates to mads sensitivity.
</commit_message>
<xml_diff>
--- a/dithionite_sensitivity/parameters.xlsx
+++ b/dithionite_sensitivity/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,156 +13,151 @@
     <sheet name="mads_tightened" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
-    <t xml:space="preserve">base</t>
-  </si>
-  <si>
-    <t xml:space="preserve">units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_s2o4_disp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_s2o4_o2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L^1.5 mol^-1.5 s^-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_s2o4_fe3 x SSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g_sed g_fe(oh)3^- s^-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">these are kept separate in the code, min and max should be multiplied by 175 for the paper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_fe2_o2_fast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g mol^-1 s^-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">factor_k_fe2_o2_slow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_fe2_o2_slow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_fe2_cr6_fast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">factor_k_fe2_cr6_slow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_fe2_cr6_slow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is2o4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifeoh3_wt%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wt %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">must convert to volume fraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifeoh3_vf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M^3/m^3_bulk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m/d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">must convert to darcy velocity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constants for VF calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rho_bulk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg/m^3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mv_feoh3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cm^3/mole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mw_feoh3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g/mole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constants for flow rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">init</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_s2o4_fe3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**cannot have fraction &gt; 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifeoh3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Factor</t>
+    <t>base</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>k_s2o4_disp</t>
+  </si>
+  <si>
+    <t>/s</t>
+  </si>
+  <si>
+    <t>k_s2o4_o2</t>
+  </si>
+  <si>
+    <t>L^1.5 mol^-1.5 s^-</t>
+  </si>
+  <si>
+    <t>k_s2o4_fe3 x SSA</t>
+  </si>
+  <si>
+    <t>g_sed g_fe(oh)3^- s^-</t>
+  </si>
+  <si>
+    <t>these are kept separate in the code, min and max should be multiplied by 175 for the paper</t>
+  </si>
+  <si>
+    <t>fraction</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>k_fe2_o2_fast</t>
+  </si>
+  <si>
+    <t>g mol^-1 s^-1</t>
+  </si>
+  <si>
+    <t>factor_k_fe2_o2_slow</t>
+  </si>
+  <si>
+    <t>k_fe2_o2_slow</t>
+  </si>
+  <si>
+    <t>k_fe2_cr6_fast</t>
+  </si>
+  <si>
+    <t>factor_k_fe2_cr6_slow</t>
+  </si>
+  <si>
+    <t>k_fe2_cr6_slow</t>
+  </si>
+  <si>
+    <t>is2o4</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>ifeoh3_wt%</t>
+  </si>
+  <si>
+    <t>Wt %</t>
+  </si>
+  <si>
+    <t>must convert to volume fraction</t>
+  </si>
+  <si>
+    <t>ifeoh3_vf</t>
+  </si>
+  <si>
+    <t>M^3/m^3_bulk</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>m/d</t>
+  </si>
+  <si>
+    <t>must convert to darcy velocity</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Constants for VF calculation</t>
+  </si>
+  <si>
+    <t>rho_bulk</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>mv_feoh3</t>
+  </si>
+  <si>
+    <t>cm^3/mole</t>
+  </si>
+  <si>
+    <t>mw_feoh3</t>
+  </si>
+  <si>
+    <t>g/mole</t>
+  </si>
+  <si>
+    <t>Constants for flow rate</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>init</t>
+  </si>
+  <si>
+    <t>k_s2o4_fe3</t>
+  </si>
+  <si>
+    <t>**cannot have fraction &gt; 1</t>
+  </si>
+  <si>
+    <t>ifeoh3</t>
+  </si>
+  <si>
+    <t>Factor</t>
   </si>
 </sst>
 </file>
@@ -170,7 +165,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
@@ -412,7 +407,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -445,7 +440,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>3.61E-005</v>
+        <v>1E-005</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
@@ -828,15 +823,15 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">LOG10(summary!B2)</f>
-        <v>-4.44249279809434</v>
+        <v>-5</v>
       </c>
       <c r="C2" s="0" t="n">
         <f aca="false">B2-1</f>
-        <v>-5.44249279809434</v>
+        <v>-6</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">B2+1</f>
-        <v>-3.44249279809434</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,7 +1032,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1070,15 +1065,15 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">LOG10(summary!B2)</f>
-        <v>-4.44249279809434</v>
+        <v>-5</v>
       </c>
       <c r="C2" s="9" t="n">
         <f aca="false">B2-F2</f>
-        <v>-4.54249279809434</v>
+        <v>-5.1</v>
       </c>
       <c r="D2" s="9" t="n">
         <f aca="false">B2+F2</f>
-        <v>-4.34249279809434</v>
+        <v>-4.9</v>
       </c>
       <c r="F2" s="7" t="n">
         <v>0.1</v>

</xml_diff>